<commit_message>
ported draft1 of data file over to dropbox
</commit_message>
<xml_diff>
--- a/data/timeline-xls_version.xlsx
+++ b/data/timeline-xls_version.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="15750" windowHeight="12045"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="15750" windowHeight="12045"/>
   </bookViews>
   <sheets>
-    <sheet name="timeline" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="timeline raw data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="105">
   <si>
     <t>&lt;h3&gt;new york times&lt;/h3&gt;&lt;h4&gt;graphics intern&lt;/h4&gt;&lt;h5&gt;dec.11-mar.12&lt;/h5&gt;&lt;p&gt;made graphics for the paper and the web&lt;/p&gt;&lt;p&gt;trained with some of the best data viz experts in the world&lt;/p&gt;&lt;p class='placeLabel'&gt;NEW YORK&lt;/p&gt;</t>
   </si>
@@ -274,6 +275,66 @@
   </si>
   <si>
     <t>taught english and did supply drops at local ngos</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;uc davis&lt;/h3&gt;&lt;h4&gt;economics major&lt;/h4&gt;&lt;h5&gt;sep. 05 to mar. 09&lt;/h5&gt;&lt;p&gt;2009: b.a. in economics&lt;/p&gt;&lt;p class='placeLabel'&gt;DAVIS, CA&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;catchafire&lt;/h3&gt;&lt;h4&gt;search marketing strategy&lt;/h4&gt;&lt;h5&gt;dec. 14 to present&lt;/h5&gt;&lt;p&gt;provide customer acquisition and analytical insights for social causes and change makers&lt;/p&gt;&lt;p class='placeLabel'&gt;SAN FRANCISCO BAY AREA&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;inflection&lt;/h3&gt;&lt;h4&gt;senior search engine marketing specialist&lt;/h4&gt;&lt;h5&gt;aug. 13 to dec. 14&lt;/h5&gt;&lt;p&gt;acquired high converting traffic via paid acquisition channels&lt;/p&gt;&lt;p&gt;optimized campaigns based on customer lifetime value&lt;/p&gt;&lt;p class='placeLabel'&gt;SAN FRANCISCO BAY AREA&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;brighter collective&lt;/h3&gt;&lt;h4&gt;media analyst&lt;/h4&gt;&lt;h5&gt;nov. 12 to aug. 13&lt;/h5&gt;&lt;p&gt;led customer acquisition search and display campaigns&lt;/p&gt;&lt;p&gt;optimized text ad copy, keywords, and built campaigns by hand&lt;/p&gt;&lt;p class='placeLabel'&gt;LOS ANGELES&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;ticketmaster&lt;/h3&gt;&lt;h4&gt;search analyst&lt;/h4&gt;&lt;h5&gt;mar. 12 to nov. 12&lt;/h5&gt;&lt;p&gt;analyzed key performance indicators for search marketing, search engine optimization, and social&lt;/p&gt;&lt;p&gt;toolbelt included adwords, sitecatalyst, and webmaster tools&lt;/p&gt;&lt;p class='placeLabel'&gt;HOLLYWOOD&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;pricegrabber&lt;/h3&gt;&lt;h4&gt;search marketing analyst&lt;/h4&gt;&lt;h5&gt;jul. 11 to mar. 12&lt;/h5&gt;&lt;p&gt;performed reporting and campaign optimizations&lt;/p&gt;&lt;p&gt;communicated daily performance results to ceo and key people&lt;/p&gt;&lt;p class='placeLabel'&gt;LOS ANGELES&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;pricegrabber&lt;/h3&gt;&lt;h4&gt;client services representative&lt;/h4&gt;&lt;h5&gt;apr. 10 to jul. 11&lt;/h5&gt;&lt;p&gt;helped clients improve ROI with pay-per-click bid suggestions&lt;/p&gt;&lt;p&gt;upped merchant participation in value-add features such as conversion tracking&lt;/p&gt;&lt;p class='placeLabel'&gt;LOS ANGELES&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;urban light&lt;/h3&gt;&lt;h4&gt;fundraising&lt;/h4&gt;&lt;h5&gt;apr. 2010 to present&lt;/h5&gt;&lt;p&gt;raise funds for a game changing organization&lt;/p&gt;&lt;p class='placeLabel'&gt;CHIANG MAI&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;human trafficking awareness orgs&lt;/h3&gt;&lt;h4&gt;awareness event planning&lt;/h4&gt;&lt;h5&gt;aug. 09 to apr. 2010&lt;/h5&gt;&lt;p&gt;planned events, screened documentaries in public venues&lt;/p&gt;&lt;p class='placeLabel'&gt;DAVIS, CA&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;the sold project&lt;/h3&gt;&lt;h4&gt;overseas volunteer&lt;/h4&gt;&lt;h5&gt;jul. 09 to aug. 09&lt;/h5&gt;&lt;p&gt;taught english and did supply drops at local ngos&lt;/p&gt;&lt;p&gt;crossed the thai - burmese border gate&lt;/p&gt;&lt;p class='placeLabel'&gt;NORTHERN THAILAND&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;various orgs&lt;/h3&gt;&lt;h4&gt;awareness event planning&lt;/h4&gt;&lt;h5&gt;mar. 09 to jul. 09&lt;/h5&gt;&lt;p&gt;worked with with a great team and planned human trafficking awareness events&lt;/p&gt;&lt;p class='placeLabel'&gt;DAVIS, CA&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>beg</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>des</t>
+  </si>
+  <si>
+    <t>undergrad</t>
+  </si>
+  <si>
+    <t>growth marketing</t>
+  </si>
+  <si>
+    <t>giving</t>
+  </si>
+  <si>
+    <t>awareness events</t>
+  </si>
+  <si>
+    <t>overseas</t>
   </si>
 </sst>
 </file>
@@ -785,13 +846,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1113,10 +1175,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="6">
+        <v>38596</v>
+      </c>
+      <c r="C2" s="6">
+        <v>39873</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="6">
+        <v>41974</v>
+      </c>
+      <c r="C3" s="6">
+        <v>42339</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="6">
+        <v>41487</v>
+      </c>
+      <c r="C4" s="6">
+        <v>41974</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="6">
+        <v>41214</v>
+      </c>
+      <c r="C5" s="6">
+        <v>41487</v>
+      </c>
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="6">
+        <v>40969</v>
+      </c>
+      <c r="C6" s="6">
+        <v>41214</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="6">
+        <v>40725</v>
+      </c>
+      <c r="C7" s="6">
+        <v>40969</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="6">
+        <v>40269</v>
+      </c>
+      <c r="C8" s="6">
+        <v>40725</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="6">
+        <v>40269</v>
+      </c>
+      <c r="C9" s="6">
+        <v>42339</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="6">
+        <v>40026</v>
+      </c>
+      <c r="C10" s="6">
+        <v>40269</v>
+      </c>
+      <c r="D10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="6">
+        <v>39995</v>
+      </c>
+      <c r="C11" s="6">
+        <v>40026</v>
+      </c>
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="6">
+        <v>39873</v>
+      </c>
+      <c r="C12" s="6">
+        <v>39995</v>
+      </c>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="B20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1128,52 +1415,52 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
@@ -1190,7 +1477,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1206,8 +1493,12 @@
       <c r="E12" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="str">
+        <f>CONCATENATE(C12,E12,D12,C13,E13,D13,C14,E14,D14,C15,E15,D15,C16,E16,D16)</f>
+        <v>&lt;h3&gt;uc davis&lt;/h3&gt;&lt;h4&gt;economics major&lt;/h4&gt;&lt;h5&gt;sep. 05 to mar. 09&lt;/h5&gt;&lt;p&gt;2009: b.a. in economics&lt;/p&gt;&lt;p class='placeLabel'&gt;DAVIS, CA&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1224,7 +1515,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1241,7 +1532,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1258,7 +1549,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1275,7 +1566,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
@@ -1291,8 +1582,12 @@
       <c r="E17" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="str">
+        <f>CONCATENATE(C17,E17,D17,C18,E18,D18,C19,E19,D19,C20,E20,D20,C21,E21,D21)</f>
+        <v>&lt;h3&gt;catchafire&lt;/h3&gt;&lt;h4&gt;search marketing strategy&lt;/h4&gt;&lt;h5&gt;dec. 14 to present&lt;/h5&gt;&lt;p&gt;provide customer acquisition and analytical insights for social causes and change makers&lt;/p&gt;&lt;p class='placeLabel'&gt;SAN FRANCISCO BAY AREA&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1309,7 +1604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1326,7 +1621,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1343,7 +1638,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1360,7 +1655,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -1376,8 +1671,12 @@
       <c r="E22" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="str">
+        <f>CONCATENATE(C22,E22,D22,C23,E23,D23,C24,E24,D24,C25,E25,D25,C26,E26,D26,C27,E27,D27)</f>
+        <v>&lt;h3&gt;inflection&lt;/h3&gt;&lt;h4&gt;senior search engine marketing specialist&lt;/h4&gt;&lt;h5&gt;aug. 13 to dec. 14&lt;/h5&gt;&lt;p&gt;acquired high converting traffic via paid acquisition channels&lt;/p&gt;&lt;p&gt;optimized campaigns based on customer lifetime value&lt;/p&gt;&lt;p class='placeLabel'&gt;SAN FRANCISCO BAY AREA&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1394,7 +1693,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1411,7 +1710,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1428,7 +1727,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1445,7 +1744,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1462,7 +1761,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>24</v>
       </c>
@@ -1478,8 +1777,12 @@
       <c r="E28" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="str">
+        <f>CONCATENATE(C28,E28,D28,C29,E29,D29,C30,E30,D30,C31,E31,D31,C32,E32,D32,C33,E33,D33)</f>
+        <v>&lt;h3&gt;brighter collective&lt;/h3&gt;&lt;h4&gt;media analyst&lt;/h4&gt;&lt;h5&gt;nov. 12 to aug. 13&lt;/h5&gt;&lt;p&gt;led customer acquisition search and display campaigns&lt;/p&gt;&lt;p&gt;optimized text ad copy, keywords, and built campaigns by hand&lt;/p&gt;&lt;p class='placeLabel'&gt;LOS ANGELES&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1496,7 +1799,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -1513,7 +1816,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1530,7 +1833,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -1547,7 +1850,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
@@ -1564,7 +1867,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>24</v>
       </c>
@@ -1580,8 +1883,12 @@
       <c r="E34" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="str">
+        <f>CONCATENATE(C34,E34,D34,C35,E35,D35,C36,E36,D36,C37,E37,D37,C38,E38,D38,C39,E39,D39)</f>
+        <v>&lt;h3&gt;ticketmaster&lt;/h3&gt;&lt;h4&gt;search analyst&lt;/h4&gt;&lt;h5&gt;mar. 12 to nov. 12&lt;/h5&gt;&lt;p&gt;analyzed key performance indicators for search marketing, search engine optimization, and social&lt;/p&gt;&lt;p&gt;toolbelt included adwords, sitecatalyst, and webmaster tools&lt;/p&gt;&lt;p class='placeLabel'&gt;HOLLYWOOD&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>24</v>
       </c>
@@ -1598,7 +1905,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
@@ -1615,7 +1922,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>24</v>
       </c>
@@ -1632,7 +1939,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>24</v>
       </c>
@@ -1649,7 +1956,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
@@ -1666,7 +1973,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>24</v>
       </c>
@@ -1682,8 +1989,12 @@
       <c r="E40" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="str">
+        <f>CONCATENATE(C40,E40,D40,C41,E41,D41,C42,E42,D42,C43,E43,D43,C44,E44,D44,C45,E45,D45)</f>
+        <v>&lt;h3&gt;pricegrabber&lt;/h3&gt;&lt;h4&gt;search marketing analyst&lt;/h4&gt;&lt;h5&gt;jul. 11 to mar. 12&lt;/h5&gt;&lt;p&gt;performed reporting and campaign optimizations&lt;/p&gt;&lt;p&gt;communicated daily performance results to ceo and key people&lt;/p&gt;&lt;p class='placeLabel'&gt;LOS ANGELES&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
@@ -1700,7 +2011,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
@@ -1717,7 +2028,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>24</v>
       </c>
@@ -1734,7 +2045,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>24</v>
       </c>
@@ -1751,7 +2062,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>24</v>
       </c>
@@ -1768,7 +2079,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>24</v>
       </c>
@@ -1784,8 +2095,12 @@
       <c r="E46" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="str">
+        <f>CONCATENATE(C46,E46,D46,C47,E47,D47,C48,E48,D48,C49,E49,D49,C50,E50,D50,C51,E51,D51)</f>
+        <v>&lt;h3&gt;pricegrabber&lt;/h3&gt;&lt;h4&gt;client services representative&lt;/h4&gt;&lt;h5&gt;apr. 10 to jul. 11&lt;/h5&gt;&lt;p&gt;helped clients improve ROI with pay-per-click bid suggestions&lt;/p&gt;&lt;p&gt;upped merchant participation in value-add features such as conversion tracking&lt;/p&gt;&lt;p class='placeLabel'&gt;LOS ANGELES&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>24</v>
       </c>
@@ -1802,7 +2117,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>24</v>
       </c>
@@ -1819,7 +2134,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
@@ -1836,7 +2151,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>24</v>
       </c>
@@ -1853,7 +2168,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>24</v>
       </c>
@@ -1870,7 +2185,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>57</v>
       </c>
@@ -1886,8 +2201,12 @@
       <c r="E52" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="1" t="str">
+        <f>CONCATENATE(C52,E52,D52,C53,E53,D53,C54,E54,D54,C55,E55,D55,C56,E56,D56)</f>
+        <v>&lt;h3&gt;urban light&lt;/h3&gt;&lt;h4&gt;fundraising&lt;/h4&gt;&lt;h5&gt;apr. 2010 to present&lt;/h5&gt;&lt;p&gt;raise funds for a game changing organization&lt;/p&gt;&lt;p class='placeLabel'&gt;CHIANG MAI&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
@@ -1904,7 +2223,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
@@ -1921,7 +2240,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
@@ -1938,7 +2257,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -1955,7 +2274,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>57</v>
       </c>
@@ -1971,8 +2290,12 @@
       <c r="E57" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="1" t="str">
+        <f>CONCATENATE(C57,E57,D57,C58,E58,D58,C59,E59,D59,C60,E60,D60,C61,E61,D61)</f>
+        <v>&lt;h3&gt;human trafficking awareness orgs&lt;/h3&gt;&lt;h4&gt;awareness event planning&lt;/h4&gt;&lt;h5&gt;aug. 09 to apr. 2010&lt;/h5&gt;&lt;p&gt;planned events, screened documentaries in public venues&lt;/p&gt;&lt;p class='placeLabel'&gt;DAVIS, CA&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -1989,7 +2312,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -2006,7 +2329,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
@@ -2023,7 +2346,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>57</v>
       </c>
@@ -2040,7 +2363,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>57</v>
       </c>
@@ -2056,8 +2379,12 @@
       <c r="E62" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="1" t="str">
+        <f>CONCATENATE(C62,E62,D62,C63,E63,D63,C64,E64,D64,C65,E65,D65,C66,E66,D66,C67,E67,D67)</f>
+        <v>&lt;h3&gt;the sold project&lt;/h3&gt;&lt;h4&gt;overseas volunteer&lt;/h4&gt;&lt;h5&gt;jul. 09 to aug. 09&lt;/h5&gt;&lt;p&gt;taught english and did supply drops at local ngos&lt;/p&gt;&lt;p&gt;crossed the thai - burmese border gate&lt;/p&gt;&lt;p class='placeLabel'&gt;NORTHERN THAILAND&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>57</v>
       </c>
@@ -2074,7 +2401,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>57</v>
       </c>
@@ -2091,7 +2418,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>57</v>
       </c>
@@ -2108,7 +2435,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>57</v>
       </c>
@@ -2125,7 +2452,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>57</v>
       </c>
@@ -2142,7 +2469,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>57</v>
       </c>
@@ -2158,8 +2485,12 @@
       <c r="E68" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="1" t="str">
+        <f>CONCATENATE(C68,E68,D68,C69,E69,D69,C70,E70,D70,C71,E71,D71,C72,E72,D72)</f>
+        <v>&lt;h3&gt;various orgs&lt;/h3&gt;&lt;h4&gt;awareness event planning&lt;/h4&gt;&lt;h5&gt;mar. 09 to jul. 09&lt;/h5&gt;&lt;p&gt;worked with with a great team and planned human trafficking awareness events&lt;/p&gt;&lt;p class='placeLabel'&gt;DAVIS, CA&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>57</v>
       </c>
@@ -2176,7 +2507,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>57</v>
       </c>
@@ -2193,7 +2524,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>57</v>
       </c>
@@ -2210,7 +2541,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>57</v>
       </c>
@@ -2227,25 +2558,25 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77" s="3"/>
       <c r="C77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B78" s="3"/>
       <c r="C78" s="2"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B79" s="3"/>
       <c r="C79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C80" s="2"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
get that scale right
</commit_message>
<xml_diff>
--- a/data/timeline-xls_version.xlsx
+++ b/data/timeline-xls_version.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="15750" windowHeight="12045"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="15750" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1188,7 +1188,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,7 +1234,7 @@
         <v>41974</v>
       </c>
       <c r="C3" s="6">
-        <v>42339</v>
+        <v>42064</v>
       </c>
       <c r="D3" t="s">
         <v>86</v>
@@ -1318,7 +1318,7 @@
         <v>40269</v>
       </c>
       <c r="C9" s="6">
-        <v>42339</v>
+        <v>42064</v>
       </c>
       <c r="D9" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
it's all set. time to post on squarespace
</commit_message>
<xml_diff>
--- a/data/timeline-xls_version.xlsx
+++ b/data/timeline-xls_version.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="15750" windowHeight="12045"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="15750" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1188,7 +1188,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1217,7 @@
         <v>97</v>
       </c>
       <c r="B2" s="6">
-        <v>38596</v>
+        <v>39783</v>
       </c>
       <c r="C2" s="6">
         <v>39873</v>
@@ -1413,7 +1413,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>